<commit_message>
Updates to BRAcACTSC and TTS
</commit_message>
<xml_diff>
--- a/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
+++ b/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BRAaCTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\trans\BRAaCTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9528938A-0C60-4F69-836B-666D774F9A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA3E91-76B2-4E00-B280-A24BBC976430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Source:</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>EV charging ports and gas pumps. We also assume this value will decline to 0 by 2050 as more EV chargers come online.</t>
+  </si>
+  <si>
+    <t>Year 2030</t>
   </si>
 </sst>
 </file>
@@ -1518,22 +1521,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="31.90625" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,216 +1544,216 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>2016</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
         <v>2021</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -1765,24 +1768,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A17B3-AFD9-42DA-AB68-E46FC6CF1D40}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1790,12 +1793,12 @@
         <v>-0.36099999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>1.268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1811,15 +1814,18 @@
         <v>-0.11600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>56</v>
       </c>
       <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1827,11 +1833,14 @@
         <v>4.12</v>
       </c>
       <c r="C8">
+        <v>4.12</v>
+      </c>
+      <c r="D8">
         <f>B8</f>
         <v>4.12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1841,8 +1850,11 @@
       <c r="C9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <v>4.12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1850,29 +1862,37 @@
         <v>68.703000000000003</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10" si="0">B10</f>
+        <f>income</f>
         <v>68.703000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f>B10</f>
+        <v>68.703000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="6">
-        <f>($B$4/$B$2*Range_EV*(1-range_ICE/Range_EV)+$B$5/$B$2*Range_EV^2*(1-range_ICE^2/Range_EV^2))*LN(income)</f>
+        <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)</f>
         <v>8.7776895901028578</v>
       </c>
       <c r="C13" s="6">
-        <f>($B$4/$B$2*C9*(1-range_ICE/C9)+$B$5/$B$2*C9^2*(1-range_ICE^2/C9^2))*LN(income)</f>
+        <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)</f>
         <v>5.8013729917508945</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="6">
+        <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -1880,7 +1900,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>0.05</v>
       </c>
@@ -1888,7 +1908,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>0.1</v>
       </c>
@@ -1896,7 +1916,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>1</v>
       </c>
@@ -1904,12 +1924,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1917,7 +1937,7 @@
         <v>120045</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1925,7 +1945,7 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1934,7 +1954,7 @@
         <v>0.1000375</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1943,29 +1963,29 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2020</v>
       </c>
@@ -1974,13 +1994,22 @@
         <v>9777.6895901028583</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
+        <v>2030</v>
+      </c>
+      <c r="B34">
+        <f>C13*1000+B26</f>
+        <v>6801.3729917508945</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>2050</v>
       </c>
-      <c r="B34">
-        <f>C13*1000</f>
-        <v>5801.3729917508945</v>
+      <c r="B35">
+        <f>D13*1000+B26</f>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1995,18 +2024,18 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2104,134 +2133,135 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" cm="1">
         <f t="array" ref="B2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!B1)</f>
-        <v>9777.6895901028765</v>
+        <v>9777.6895901027601</v>
       </c>
       <c r="C2" s="3" cm="1">
         <f t="array" ref="C2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!C1)</f>
-        <v>9645.1457034911145</v>
+        <v>9480.0579302676488</v>
       </c>
       <c r="D2" s="3" cm="1">
         <f t="array" ref="D2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!D1)</f>
-        <v>9512.6018168794108</v>
+        <v>9182.426270432421</v>
       </c>
       <c r="E2" s="3" cm="1">
         <f t="array" ref="E2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!E1)</f>
-        <v>9380.0579302676488</v>
+        <v>8884.7946105971932</v>
       </c>
       <c r="F2" s="3" cm="1">
         <f t="array" ref="F2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!F1)</f>
-        <v>9247.514043655945</v>
+        <v>8587.1629507620819</v>
       </c>
       <c r="G2" s="3" cm="1">
         <f t="array" ref="G2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!G1)</f>
-        <v>9114.970157044183</v>
+        <v>8289.5312909268541</v>
       </c>
       <c r="H2" s="3" cm="1">
         <f t="array" ref="H2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!H1)</f>
-        <v>8982.4262704324792</v>
+        <v>7991.8996310916264</v>
       </c>
       <c r="I2" s="3" cm="1">
         <f t="array" ref="I2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!I1)</f>
-        <v>8849.8823838207172</v>
+        <v>7694.2679712563986</v>
       </c>
       <c r="J2" s="3" cm="1">
         <f t="array" ref="J2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!J1)</f>
-        <v>8717.3384972090134</v>
+        <v>7396.6363114212872</v>
       </c>
       <c r="K2" s="3" cm="1">
         <f t="array" ref="K2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!K1)</f>
-        <v>8584.7946105972514</v>
+        <v>7099.0046515860595</v>
       </c>
       <c r="L2" s="3" cm="1">
         <f t="array" ref="L2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!L1)</f>
-        <v>8452.2507239855477</v>
+        <v>6801.3729917508317</v>
       </c>
       <c r="M2" s="3" cm="1">
-        <f t="array" ref="M2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!M1)</f>
-        <v>8319.7068373737857</v>
+        <f t="array" ref="M2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!M1)</f>
+        <v>6511.3043421633774</v>
       </c>
       <c r="N2" s="3" cm="1">
-        <f t="array" ref="N2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!N1)</f>
-        <v>8187.1629507620819</v>
+        <f t="array" ref="N2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!N1)</f>
+        <v>6221.2356925758068</v>
       </c>
       <c r="O2" s="3" cm="1">
-        <f t="array" ref="O2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!O1)</f>
-        <v>8054.6190641503199</v>
+        <f t="array" ref="O2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!O1)</f>
+        <v>5931.1670429883525</v>
       </c>
       <c r="P2" s="3" cm="1">
-        <f t="array" ref="P2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!P1)</f>
-        <v>7922.0751775386161</v>
+        <f t="array" ref="P2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!P1)</f>
+        <v>5641.0983934007818</v>
       </c>
       <c r="Q2" s="3" cm="1">
-        <f t="array" ref="Q2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!Q1)</f>
-        <v>7789.5312909268541</v>
+        <f t="array" ref="Q2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Q1)</f>
+        <v>5351.0297438132111</v>
       </c>
       <c r="R2" s="3" cm="1">
-        <f t="array" ref="R2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!R1)</f>
-        <v>7656.9874043151503</v>
+        <f t="array" ref="R2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!R1)</f>
+        <v>5060.9610942256404</v>
       </c>
       <c r="S2" s="3" cm="1">
-        <f t="array" ref="S2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!S1)</f>
-        <v>7524.4435177033884</v>
+        <f t="array" ref="S2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!S1)</f>
+        <v>4770.8924446381861</v>
       </c>
       <c r="T2" s="3" cm="1">
-        <f t="array" ref="T2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!T1)</f>
-        <v>7391.8996310916846</v>
+        <f t="array" ref="T2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!T1)</f>
+        <v>4480.8237950506154</v>
       </c>
       <c r="U2" s="3" cm="1">
-        <f t="array" ref="U2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!U1)</f>
-        <v>7259.3557444799226</v>
+        <f t="array" ref="U2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!U1)</f>
+        <v>4190.7551454630448</v>
       </c>
       <c r="V2" s="3" cm="1">
-        <f t="array" ref="V2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!V1)</f>
-        <v>7126.8118578682188</v>
+        <f t="array" ref="V2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!V1)</f>
+        <v>3900.6864958754741</v>
       </c>
       <c r="W2" s="3" cm="1">
-        <f t="array" ref="W2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!W1)</f>
-        <v>6994.2679712564568</v>
+        <f t="array" ref="W2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!W1)</f>
+        <v>3610.6178462879034</v>
       </c>
       <c r="X2" s="3" cm="1">
-        <f t="array" ref="X2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!X1)</f>
-        <v>6861.724084644753</v>
+        <f t="array" ref="X2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!X1)</f>
+        <v>3320.5491967004491</v>
       </c>
       <c r="Y2" s="3" cm="1">
-        <f t="array" ref="Y2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!Y1)</f>
-        <v>6729.180198032991</v>
+        <f t="array" ref="Y2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Y1)</f>
+        <v>3030.4805471128784</v>
       </c>
       <c r="Z2" s="3" cm="1">
-        <f t="array" ref="Z2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!Z1)</f>
-        <v>6596.6363114212872</v>
+        <f t="array" ref="Z2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Z1)</f>
+        <v>2740.4118975253077</v>
       </c>
       <c r="AA2" s="3" cm="1">
-        <f t="array" ref="AA2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AA1)</f>
-        <v>6464.0924248095253</v>
+        <f t="array" ref="AA2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AA1)</f>
+        <v>2450.343247937737</v>
       </c>
       <c r="AB2" s="3" cm="1">
-        <f t="array" ref="AB2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AB1)</f>
-        <v>6331.5485381978215</v>
+        <f t="array" ref="AB2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AB1)</f>
+        <v>2160.2745983502828</v>
       </c>
       <c r="AC2" s="3" cm="1">
-        <f t="array" ref="AC2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AC1)</f>
-        <v>6199.0046515860595</v>
+        <f t="array" ref="AC2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AC1)</f>
+        <v>1870.2059487627121</v>
       </c>
       <c r="AD2" s="3" cm="1">
-        <f t="array" ref="AD2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AD1)</f>
-        <v>6066.4607649743557</v>
+        <f t="array" ref="AD2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AD1)</f>
+        <v>1580.1372991751414</v>
       </c>
       <c r="AE2" s="3" cm="1">
-        <f t="array" ref="AE2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AE1)</f>
-        <v>5933.9168783626519</v>
+        <f t="array" ref="AE2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AE1)</f>
+        <v>1290.0686495875707</v>
       </c>
       <c r="AF2" s="3" cm="1">
-        <f t="array" ref="AF2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!AF1)</f>
-        <v>5801.3729917508899</v>
-      </c>
+        <f t="array" ref="AF2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AF1)</f>
+        <v>1000</v>
+      </c>
+      <c r="AG2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adjust for inflation in BRAsCTSC
</commit_message>
<xml_diff>
--- a/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
+++ b/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\trans\BRAaCTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BRAaCTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA3E91-76B2-4E00-B280-A24BBC976430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2A0F01-9494-484D-88C4-D1ADDBE760E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="Range_EV">Calculations!$B$9</definedName>
     <definedName name="range_ICE">Calculations!$B$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Source:</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>Year 2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2020 median range taken from historical data. 2030 and 2050 are estimated, with the 2050 </t>
+  </si>
+  <si>
+    <t>range roughly corresponding to today's maximum range</t>
   </si>
 </sst>
 </file>
@@ -258,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +274,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -298,10 +320,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,8 +338,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,7 +449,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Calculations!$A$16:$A$19</c:f>
+              <c:f>Calculations!$A$17:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -444,7 +470,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Calculations!$B$16:$B$19</c:f>
+              <c:f>Calculations!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1225,7 +1251,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1521,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1717,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B38" s="9" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1762,21 +1788,24 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B38" r:id="rId1" xr:uid="{14EF0A86-0973-41E2-9D23-51C96C77958E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A17B3-AFD9-42DA-AB68-E46FC6CF1D40}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1847,10 +1876,10 @@
       <c r="B9">
         <v>2.59</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>4.12</v>
       </c>
     </row>
@@ -1861,155 +1890,165 @@
       <c r="B10">
         <v>68.703000000000003</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <f>income</f>
         <v>68.703000000000003</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <f>B10</f>
         <v>68.703000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6">
-        <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)</f>
-        <v>8.7776895901028578</v>
-      </c>
-      <c r="C13" s="6">
-        <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)</f>
-        <v>5.8013729917508945</v>
-      </c>
-      <c r="D13" s="6">
-        <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)</f>
+      <c r="B14" s="6">
+        <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)*About!$B$53</f>
+        <v>7.8828464065137096</v>
+      </c>
+      <c r="C14" s="6">
+        <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)*About!$B$53</f>
+        <v>5.2099509525186276</v>
+      </c>
+      <c r="D14" s="6">
+        <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)*About!$B$53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>7500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>0.05</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1750</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>0.1</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>1</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>120045</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>30</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>1200000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>31</v>
       </c>
-      <c r="B25">
-        <f>B23/B24</f>
+      <c r="B26">
+        <f>B24/B25</f>
         <v>0.1000375</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>32</v>
       </c>
-      <c r="B26">
-        <f>B18</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B27">
+        <f>B19*About!$B$53</f>
+        <v>898.05481563188175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>2020</v>
       </c>
-      <c r="B33">
-        <f>B13*1000+B26</f>
-        <v>9777.6895901028583</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B34">
+        <f>B14*1000+B27</f>
+        <v>8780.9012221455905</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
         <v>2030</v>
       </c>
-      <c r="B34">
-        <f>C13*1000+B26</f>
-        <v>6801.3729917508945</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B35">
+        <f>C14*1000+B27</f>
+        <v>6108.0057681505095</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2050</v>
       </c>
-      <c r="B35">
-        <f>D13*1000+B26</f>
-        <v>1000</v>
+      <c r="B36">
+        <f>D14*1000+B27</f>
+        <v>898.05481563188175</v>
       </c>
     </row>
   </sheetData>
@@ -2026,8 +2065,8 @@
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,128 +2177,128 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" cm="1">
-        <f t="array" ref="B2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!B1)</f>
-        <v>9777.6895901027601</v>
+        <f t="array" ref="B2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!B1)</f>
+        <v>8780.9012221456505</v>
       </c>
       <c r="C2" s="3" cm="1">
-        <f t="array" ref="C2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!C1)</f>
-        <v>9480.0579302676488</v>
+        <f t="array" ref="C2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!C1)</f>
+        <v>8513.6116767461644</v>
       </c>
       <c r="D2" s="3" cm="1">
-        <f t="array" ref="D2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!D1)</f>
-        <v>9182.426270432421</v>
+        <f t="array" ref="D2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!D1)</f>
+        <v>8246.3221313466784</v>
       </c>
       <c r="E2" s="3" cm="1">
-        <f t="array" ref="E2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!E1)</f>
-        <v>8884.7946105971932</v>
+        <f t="array" ref="E2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!E1)</f>
+        <v>7979.0325859471923</v>
       </c>
       <c r="F2" s="3" cm="1">
-        <f t="array" ref="F2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!F1)</f>
-        <v>8587.1629507620819</v>
+        <f t="array" ref="F2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!F1)</f>
+        <v>7711.7430405477062</v>
       </c>
       <c r="G2" s="3" cm="1">
-        <f t="array" ref="G2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!G1)</f>
-        <v>8289.5312909268541</v>
+        <f t="array" ref="G2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!G1)</f>
+        <v>7444.4534951481037</v>
       </c>
       <c r="H2" s="3" cm="1">
-        <f t="array" ref="H2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!H1)</f>
-        <v>7991.8996310916264</v>
+        <f t="array" ref="H2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!H1)</f>
+        <v>7177.1639497486176</v>
       </c>
       <c r="I2" s="3" cm="1">
-        <f t="array" ref="I2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!I1)</f>
-        <v>7694.2679712563986</v>
+        <f t="array" ref="I2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!I1)</f>
+        <v>6909.8744043491315</v>
       </c>
       <c r="J2" s="3" cm="1">
-        <f t="array" ref="J2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!J1)</f>
-        <v>7396.6363114212872</v>
+        <f t="array" ref="J2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!J1)</f>
+        <v>6642.5848589496454</v>
       </c>
       <c r="K2" s="3" cm="1">
-        <f t="array" ref="K2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!K1)</f>
-        <v>7099.0046515860595</v>
+        <f t="array" ref="K2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!K1)</f>
+        <v>6375.2953135501593</v>
       </c>
       <c r="L2" s="3" cm="1">
-        <f t="array" ref="L2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!L1)</f>
-        <v>6801.3729917508317</v>
+        <f t="array" ref="L2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!L1)</f>
+        <v>6108.0057681505568</v>
       </c>
       <c r="M2" s="3" cm="1">
-        <f t="array" ref="M2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!M1)</f>
-        <v>6511.3043421633774</v>
+        <f t="array" ref="M2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!M1)</f>
+        <v>5847.5082205246435</v>
       </c>
       <c r="N2" s="3" cm="1">
-        <f t="array" ref="N2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!N1)</f>
-        <v>6221.2356925758068</v>
+        <f t="array" ref="N2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!N1)</f>
+        <v>5587.0106728986138</v>
       </c>
       <c r="O2" s="3" cm="1">
-        <f t="array" ref="O2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!O1)</f>
-        <v>5931.1670429883525</v>
+        <f t="array" ref="O2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!O1)</f>
+        <v>5326.5131252727006</v>
       </c>
       <c r="P2" s="3" cm="1">
-        <f t="array" ref="P2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!P1)</f>
-        <v>5641.0983934007818</v>
+        <f t="array" ref="P2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!P1)</f>
+        <v>5066.0155776467873</v>
       </c>
       <c r="Q2" s="3" cm="1">
-        <f t="array" ref="Q2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Q1)</f>
-        <v>5351.0297438132111</v>
+        <f t="array" ref="Q2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Q1)</f>
+        <v>4805.518030020874</v>
       </c>
       <c r="R2" s="3" cm="1">
-        <f t="array" ref="R2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!R1)</f>
-        <v>5060.9610942256404</v>
+        <f t="array" ref="R2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!R1)</f>
+        <v>4545.0204823949607</v>
       </c>
       <c r="S2" s="3" cm="1">
-        <f t="array" ref="S2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!S1)</f>
-        <v>4770.8924446381861</v>
+        <f t="array" ref="S2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!S1)</f>
+        <v>4284.5229347690474</v>
       </c>
       <c r="T2" s="3" cm="1">
-        <f t="array" ref="T2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!T1)</f>
-        <v>4480.8237950506154</v>
+        <f t="array" ref="T2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!T1)</f>
+        <v>4024.0253871431341</v>
       </c>
       <c r="U2" s="3" cm="1">
-        <f t="array" ref="U2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!U1)</f>
-        <v>4190.7551454630448</v>
+        <f t="array" ref="U2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!U1)</f>
+        <v>3763.5278395171044</v>
       </c>
       <c r="V2" s="3" cm="1">
-        <f t="array" ref="V2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!V1)</f>
-        <v>3900.6864958754741</v>
+        <f t="array" ref="V2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!V1)</f>
+        <v>3503.0302918911912</v>
       </c>
       <c r="W2" s="3" cm="1">
-        <f t="array" ref="W2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!W1)</f>
-        <v>3610.6178462879034</v>
+        <f t="array" ref="W2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!W1)</f>
+        <v>3242.5327442652779</v>
       </c>
       <c r="X2" s="3" cm="1">
-        <f t="array" ref="X2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!X1)</f>
-        <v>3320.5491967004491</v>
+        <f t="array" ref="X2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!X1)</f>
+        <v>2982.0351966393646</v>
       </c>
       <c r="Y2" s="3" cm="1">
-        <f t="array" ref="Y2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Y1)</f>
-        <v>3030.4805471128784</v>
+        <f t="array" ref="Y2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Y1)</f>
+        <v>2721.5376490134513</v>
       </c>
       <c r="Z2" s="3" cm="1">
-        <f t="array" ref="Z2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Z1)</f>
-        <v>2740.4118975253077</v>
+        <f t="array" ref="Z2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Z1)</f>
+        <v>2461.040101387538</v>
       </c>
       <c r="AA2" s="3" cm="1">
-        <f t="array" ref="AA2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AA1)</f>
-        <v>2450.343247937737</v>
+        <f t="array" ref="AA2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AA1)</f>
+        <v>2200.5425537615083</v>
       </c>
       <c r="AB2" s="3" cm="1">
-        <f t="array" ref="AB2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AB1)</f>
-        <v>2160.2745983502828</v>
+        <f t="array" ref="AB2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AB1)</f>
+        <v>1940.045006135595</v>
       </c>
       <c r="AC2" s="3" cm="1">
-        <f t="array" ref="AC2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AC1)</f>
-        <v>1870.2059487627121</v>
+        <f t="array" ref="AC2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AC1)</f>
+        <v>1679.5474585096817</v>
       </c>
       <c r="AD2" s="3" cm="1">
-        <f t="array" ref="AD2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AD1)</f>
-        <v>1580.1372991751414</v>
+        <f t="array" ref="AD2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AD1)</f>
+        <v>1419.0499108837685</v>
       </c>
       <c r="AE2" s="3" cm="1">
-        <f t="array" ref="AE2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AE1)</f>
-        <v>1290.0686495875707</v>
+        <f t="array" ref="AE2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AE1)</f>
+        <v>1158.5523632578552</v>
       </c>
       <c r="AF2" s="3" cm="1">
-        <f t="array" ref="AF2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AF1)</f>
-        <v>1000</v>
+        <f t="array" ref="AF2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AF1)</f>
+        <v>898.05481563194189</v>
       </c>
       <c r="AG2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Use IIJA funding to customize EV charger assumptions in trans/BRAaCTSC
</commit_message>
<xml_diff>
--- a/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
+++ b/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BRAaCTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2A0F01-9494-484D-88C4-D1ADDBE760E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02F20B-346B-4E17-A776-81D370EAD24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="BRAaCTSC" sheetId="3" r:id="rId3"/>
+    <sheet name="EV charger assumptions" sheetId="5" r:id="rId3"/>
+    <sheet name="BRAaCTSC" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="income">Calculations!$B$10</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Source:</t>
   </si>
@@ -152,9 +153,6 @@
     <t>https://www.nrel.gov/docs/fy13osti/55639.pdf</t>
   </si>
   <si>
-    <t>EVSE ports:</t>
-  </si>
-  <si>
     <t>Number of gas pumps</t>
   </si>
   <si>
@@ -233,12 +231,6 @@
     <t>Calculations</t>
   </si>
   <si>
-    <t>Year 2020</t>
-  </si>
-  <si>
-    <t>Year 2050</t>
-  </si>
-  <si>
     <t xml:space="preserve">250 miles and is forecated to continue improving. Therefore, we start with today's median range, and assume </t>
   </si>
   <si>
@@ -248,13 +240,31 @@
     <t>EV charging ports and gas pumps. We also assume this value will decline to 0 by 2050 as more EV chargers come online.</t>
   </si>
   <si>
-    <t>Year 2030</t>
-  </si>
-  <si>
     <t xml:space="preserve">*2020 median range taken from historical data. 2030 and 2050 are estimated, with the 2050 </t>
   </si>
   <si>
     <t>range roughly corresponding to today's maximum range</t>
+  </si>
+  <si>
+    <t>We assume EV charger additions based on investments in the Infrastructure Investment and Jobs Act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total government funding: </t>
+  </si>
+  <si>
+    <t>($7.5 billion between 2022 and 2026), assuming 80% of the costs are paid for by the government.</t>
+  </si>
+  <si>
+    <t>Total government + private funding:</t>
+  </si>
+  <si>
+    <t>Average weighted charger cost (see trans/EVCC):</t>
+  </si>
+  <si>
+    <t>Chargers added by 2026:</t>
+  </si>
+  <si>
+    <t>2020 EVSE ports:</t>
   </si>
 </sst>
 </file>
@@ -324,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -340,6 +350,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -445,7 +458,43 @@
             </c:spPr>
             <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8828958880139982E-2"/>
+                  <c:y val="-0.13703885898644008"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1548,7 +1597,7 @@
   <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A51" sqref="A51:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,12 +1667,12 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1633,22 +1682,22 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
@@ -1658,17 +1707,17 @@
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -1683,27 +1732,27 @@
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,12 +1762,12 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,42 +1790,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1797,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A17B3-AFD9-42DA-AB68-E46FC6CF1D40}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,19 +1893,19 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7">
+        <v>2030</v>
+      </c>
+      <c r="D7">
+        <v>2050</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>4.12</v>
@@ -1901,12 +1950,12 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,7 +1980,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -1939,7 +1988,7 @@
         <v>7500</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>0.05</v>
       </c>
@@ -1947,7 +1996,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>0.1</v>
       </c>
@@ -1955,7 +2004,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>1</v>
       </c>
@@ -1963,92 +2012,137 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="B24">
         <v>120045</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25">
         <v>1200000</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2020</v>
+      </c>
+      <c r="C27">
+        <v>2027</v>
+      </c>
+      <c r="D27">
+        <v>2030</v>
+      </c>
+      <c r="E27">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
         <f>B24/B25</f>
         <v>0.1000375</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27">
+      <c r="C28">
+        <f>(B24+'EV charger assumptions'!B9)/Calculations!B25</f>
+        <v>0.41965865943214825</v>
+      </c>
+      <c r="D28">
+        <f>(E28-C28)/(E27-C27)*3+C28</f>
+        <v>0.495355356027955</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
         <f>B19*About!$B$53</f>
         <v>898.05481563188175</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="C29">
+        <f>-667.1*LN(C28)-241.23</f>
+        <v>338.02201174921117</v>
+      </c>
+      <c r="D29">
+        <f>-667.1*LN(D28)-241.23</f>
+        <v>227.39432995486422</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2020</v>
-      </c>
-      <c r="B34">
-        <f>B14*1000+B27</f>
-        <v>8780.9012221455905</v>
-      </c>
-    </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2030</v>
-      </c>
-      <c r="B35">
-        <f>C14*1000+B27</f>
-        <v>6108.0057681505095</v>
-      </c>
+      <c r="A35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
+        <v>2020</v>
+      </c>
+      <c r="B36">
+        <f>B14*1000+B29</f>
+        <v>8780.9012221455905</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2027</v>
+      </c>
+      <c r="B37" cm="1">
+        <f t="array" ref="B37">TREND(B14:C14,B7:C7,C27)*1000+C29</f>
+        <v>6349.8416004663277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2030</v>
+      </c>
+      <c r="B38">
+        <f>C14*1000+D29</f>
+        <v>5437.3452824734923</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>2050</v>
       </c>
-      <c r="B36">
-        <f>D14*1000+B27</f>
-        <v>898.05481563188175</v>
+      <c r="B39">
+        <f>D14*1000+E29</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2059,6 +2153,69 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D98A39-3A78-451F-9516-0CF8624C92E2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>7500000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <f>B4/0.8</f>
+        <v>9375000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>24443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B5/B7</f>
+        <v>383545.39131857792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -2066,7 +2223,7 @@
   <dimension ref="A1:AG2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2177,128 +2334,128 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" cm="1">
-        <f t="array" ref="B2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!B1)</f>
+        <f t="array" ref="B2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!B1)</f>
         <v>8780.9012221456505</v>
       </c>
       <c r="C2" s="3" cm="1">
-        <f t="array" ref="C2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!C1)</f>
-        <v>8513.6116767461644</v>
+        <f t="array" ref="C2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!C1)</f>
+        <v>8433.6069904771866</v>
       </c>
       <c r="D2" s="3" cm="1">
-        <f t="array" ref="D2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!D1)</f>
-        <v>8246.3221313466784</v>
+        <f t="array" ref="D2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!D1)</f>
+        <v>8086.3127588086063</v>
       </c>
       <c r="E2" s="3" cm="1">
-        <f t="array" ref="E2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!E1)</f>
-        <v>7979.0325859471923</v>
+        <f t="array" ref="E2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!E1)</f>
+        <v>7739.0185271401424</v>
       </c>
       <c r="F2" s="3" cm="1">
-        <f t="array" ref="F2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!F1)</f>
-        <v>7711.7430405477062</v>
+        <f t="array" ref="F2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!F1)</f>
+        <v>7391.7242954716785</v>
       </c>
       <c r="G2" s="3" cm="1">
-        <f t="array" ref="G2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!G1)</f>
-        <v>7444.4534951481037</v>
+        <f t="array" ref="G2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!G1)</f>
+        <v>7044.4300638032146</v>
       </c>
       <c r="H2" s="3" cm="1">
-        <f t="array" ref="H2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!H1)</f>
-        <v>7177.1639497486176</v>
+        <f t="array" ref="H2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!H1)</f>
+        <v>6697.1358321347507</v>
       </c>
       <c r="I2" s="3" cm="1">
-        <f t="array" ref="I2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!I1)</f>
-        <v>6909.8744043491315</v>
+        <f t="array" ref="I2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!I1)</f>
+        <v>6349.8416004662868</v>
       </c>
       <c r="J2" s="3" cm="1">
-        <f t="array" ref="J2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!J1)</f>
-        <v>6642.5848589496454</v>
+        <f t="array" ref="J2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!J1)</f>
+        <v>6045.6761611354304</v>
       </c>
       <c r="K2" s="3" cm="1">
-        <f t="array" ref="K2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!K1)</f>
-        <v>6375.2953135501593</v>
+        <f t="array" ref="K2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!K1)</f>
+        <v>5741.5107218045741</v>
       </c>
       <c r="L2" s="3" cm="1">
-        <f t="array" ref="L2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!L1)</f>
-        <v>6108.0057681505568</v>
+        <f t="array" ref="L2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!L1)</f>
+        <v>5437.3452824736014</v>
       </c>
       <c r="M2" s="3" cm="1">
-        <f t="array" ref="M2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!M1)</f>
-        <v>5847.5082205246435</v>
+        <f t="array" ref="M2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!M1)</f>
+        <v>5165.4780183498515</v>
       </c>
       <c r="N2" s="3" cm="1">
-        <f t="array" ref="N2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!N1)</f>
-        <v>5587.0106728986138</v>
+        <f t="array" ref="N2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!N1)</f>
+        <v>4893.610754226218</v>
       </c>
       <c r="O2" s="3" cm="1">
-        <f t="array" ref="O2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!O1)</f>
-        <v>5326.5131252727006</v>
+        <f t="array" ref="O2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!O1)</f>
+        <v>4621.7434901024681</v>
       </c>
       <c r="P2" s="3" cm="1">
-        <f t="array" ref="P2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!P1)</f>
-        <v>5066.0155776467873</v>
+        <f t="array" ref="P2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!P1)</f>
+        <v>4349.8762259788346</v>
       </c>
       <c r="Q2" s="3" cm="1">
-        <f t="array" ref="Q2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Q1)</f>
-        <v>4805.518030020874</v>
+        <f t="array" ref="Q2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Q1)</f>
+        <v>4078.0089618552011</v>
       </c>
       <c r="R2" s="3" cm="1">
-        <f t="array" ref="R2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!R1)</f>
-        <v>4545.0204823949607</v>
+        <f t="array" ref="R2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!R1)</f>
+        <v>3806.1416977314511</v>
       </c>
       <c r="S2" s="3" cm="1">
-        <f t="array" ref="S2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!S1)</f>
-        <v>4284.5229347690474</v>
+        <f t="array" ref="S2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!S1)</f>
+        <v>3534.2744336078176</v>
       </c>
       <c r="T2" s="3" cm="1">
-        <f t="array" ref="T2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!T1)</f>
-        <v>4024.0253871431341</v>
+        <f t="array" ref="T2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!T1)</f>
+        <v>3262.4071694841841</v>
       </c>
       <c r="U2" s="3" cm="1">
-        <f t="array" ref="U2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!U1)</f>
-        <v>3763.5278395171044</v>
+        <f t="array" ref="U2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!U1)</f>
+        <v>2990.5399053604342</v>
       </c>
       <c r="V2" s="3" cm="1">
-        <f t="array" ref="V2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!V1)</f>
-        <v>3503.0302918911912</v>
+        <f t="array" ref="V2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!V1)</f>
+        <v>2718.6726412368007</v>
       </c>
       <c r="W2" s="3" cm="1">
-        <f t="array" ref="W2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!W1)</f>
-        <v>3242.5327442652779</v>
+        <f t="array" ref="W2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!W1)</f>
+        <v>2446.8053771130508</v>
       </c>
       <c r="X2" s="3" cm="1">
-        <f t="array" ref="X2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!X1)</f>
-        <v>2982.0351966393646</v>
+        <f t="array" ref="X2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!X1)</f>
+        <v>2174.9381129894173</v>
       </c>
       <c r="Y2" s="3" cm="1">
-        <f t="array" ref="Y2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Y1)</f>
-        <v>2721.5376490134513</v>
+        <f t="array" ref="Y2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Y1)</f>
+        <v>1903.0708488657838</v>
       </c>
       <c r="Z2" s="3" cm="1">
-        <f t="array" ref="Z2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!Z1)</f>
-        <v>2461.040101387538</v>
+        <f t="array" ref="Z2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Z1)</f>
+        <v>1631.2035847420339</v>
       </c>
       <c r="AA2" s="3" cm="1">
-        <f t="array" ref="AA2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AA1)</f>
-        <v>2200.5425537615083</v>
+        <f t="array" ref="AA2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AA1)</f>
+        <v>1359.3363206184004</v>
       </c>
       <c r="AB2" s="3" cm="1">
-        <f t="array" ref="AB2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AB1)</f>
-        <v>1940.045006135595</v>
+        <f t="array" ref="AB2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AB1)</f>
+        <v>1087.4690564947668</v>
       </c>
       <c r="AC2" s="3" cm="1">
-        <f t="array" ref="AC2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AC1)</f>
-        <v>1679.5474585096817</v>
+        <f t="array" ref="AC2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AC1)</f>
+        <v>815.60179237101693</v>
       </c>
       <c r="AD2" s="3" cm="1">
-        <f t="array" ref="AD2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AD1)</f>
-        <v>1419.0499108837685</v>
+        <f t="array" ref="AD2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AD1)</f>
+        <v>543.73452824738342</v>
       </c>
       <c r="AE2" s="3" cm="1">
-        <f t="array" ref="AE2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AE1)</f>
-        <v>1158.5523632578552</v>
+        <f t="array" ref="AE2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AE1)</f>
+        <v>271.86726412374992</v>
       </c>
       <c r="AF2" s="3" cm="1">
-        <f t="array" ref="AF2">TREND(Calculations!$B$35:$B$36,Calculations!$A$35:$A$36,BRAaCTSC!AF1)</f>
-        <v>898.05481563194189</v>
+        <f t="array" ref="AF2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AF1)</f>
+        <v>0</v>
       </c>
       <c r="AG2" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updates to incorporate IRA forestry and EV charger calculations into BAU
</commit_message>
<xml_diff>
--- a/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
+++ b/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BRAaCTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02F20B-346B-4E17-A776-81D370EAD24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6D8A9C-75C3-4197-8A87-AD6FE516D6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="EV charger assumptions" sheetId="5" r:id="rId3"/>
-    <sheet name="BRAaCTSC" sheetId="3" r:id="rId4"/>
+    <sheet name="IIJA" sheetId="5" r:id="rId3"/>
+    <sheet name="Inflation Reduction Act" sheetId="6" r:id="rId4"/>
+    <sheet name="BRAaCTSC" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="income">Calculations!$B$10</definedName>
     <definedName name="Range_EV">Calculations!$B$9</definedName>
     <definedName name="range_ICE">Calculations!$B$8</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
   <si>
     <t>Source:</t>
   </si>
@@ -264,7 +265,65 @@
     <t>Chargers added by 2026:</t>
   </si>
   <si>
-    <t>2020 EVSE ports:</t>
+    <t>Methodology:</t>
+  </si>
+  <si>
+    <t>Calculations:</t>
+  </si>
+  <si>
+    <t>Alternative fuel refueling property credit amount</t>
+  </si>
+  <si>
+    <t>Assumed Amount of Spending Directed Toward Public LDV Chargers</t>
+  </si>
+  <si>
+    <t>Number of Chargers Added</t>
+  </si>
+  <si>
+    <t>Chargers Added by 2032</t>
+  </si>
+  <si>
+    <t>We calculate an incremental number of chargers deployed based on funding in the Inflation Reduction Act and the model's weighted average charger cost. We take estimated funding from the released JCT scores and assume 80% of the spending is directed toward public chargers. We do not attempt to model the effects of private chargers. The number of additional chargers is then fed into the shadow price used to represent range/charging anxiety for passenger LDV owners, which is partially determined by the ratio of charging infrastructure to gasoline pumps. This adjustment helps to drop the shadow price in response to additional infrastructure and increase consumer adoption of electric vehicles.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri, sans-serif"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri, sans-serif"/>
+      </rPr>
+      <t>https://www.jct.gov/publications/2022/jcx-18-22/</t>
+    </r>
+  </si>
+  <si>
+    <t>EPS Weighted Avg Charger Cost (see trans/EVCC):</t>
+  </si>
+  <si>
+    <t>2022 to 2012 $</t>
+  </si>
+  <si>
+    <t>JCT Estimates for Alternative fuel refueling property credit (million 2022$)</t>
+  </si>
+  <si>
+    <t>Assumed Number of EVSE ports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We adjust our calculations by an estimated number of public charger additions from both the Infrastructure Investment and Jobs Act </t>
+  </si>
+  <si>
+    <t>and the Inflation Reduction Act (see tabs for methodology).</t>
+  </si>
+  <si>
+    <t>Government Outlays After Transferability Multiplier of 7.5%</t>
   </si>
 </sst>
 </file>
@@ -274,7 +333,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +365,60 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF1155CC"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri, sans-serif"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +431,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -330,11 +447,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -342,7 +460,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -353,10 +470,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3 2" xfId="2" xr:uid="{3F0B3957-5839-491A-BB84-14323CF38870}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1594,246 +1734,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="B4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="8">
+    <row r="5" spans="1:2">
+      <c r="B5" s="7">
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="B6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="B7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="1:2">
+      <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="B11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
+    <row r="12" spans="1:2">
+      <c r="B12" s="7">
         <v>2013</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="B13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
+    <row r="15" spans="1:2">
+      <c r="B15" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="B16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+    <row r="17" spans="2:2">
+      <c r="B17" s="7">
         <v>2018</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="2:2">
+      <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="8">
+    <row r="23" spans="2:2">
+      <c r="B23" s="7">
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2">
       <c r="B24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="7" t="s">
+    <row r="27" spans="2:2">
+      <c r="B27" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="8">
+    <row r="29" spans="2:2">
+      <c r="B29" s="7">
         <v>2016</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2">
       <c r="B30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2">
       <c r="B32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+    <row r="34" spans="1:2">
+      <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="B35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="8">
+    <row r="36" spans="1:2">
+      <c r="B36" s="7">
         <v>2021</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="B37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+    <row r="38" spans="1:2">
+      <c r="B38" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>25</v>
       </c>
       <c r="B53">
         <v>0.89805481563188172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1846,24 +1996,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A17B3-AFD9-42DA-AB68-E46FC6CF1D40}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1871,12 +2022,12 @@
         <v>-0.36099999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1884,7 +2035,7 @@
         <v>1.268</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1892,7 +2043,7 @@
         <v>-0.11600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="B7">
         <v>2020</v>
       </c>
@@ -1903,7 +2054,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1918,230 +2069,243 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>2.59</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>3</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>4.12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <v>68.703000000000003</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <f>income</f>
         <v>68.703000000000003</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f>B10</f>
         <v>68.703000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)*About!$B$53</f>
         <v>7.8828464065137096</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)*About!$B$53</f>
         <v>5.2099509525186276</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)*About!$B$53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="17" spans="1:5">
+      <c r="A17" s="5">
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="B17">
         <v>7500</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="18" spans="1:5">
+      <c r="A18" s="5">
         <v>0.05</v>
       </c>
       <c r="B18">
         <v>1750</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="19" spans="1:5">
+      <c r="A19" s="5">
         <v>0.1</v>
       </c>
       <c r="B19">
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="20" spans="1:5">
+      <c r="A20" s="5">
         <v>1</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="B24">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>2020</v>
+      </c>
+      <c r="B27">
         <v>120045</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>2050</v>
+      </c>
+      <c r="B28">
         <v>1200000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27">
+    <row r="30" spans="1:5">
+      <c r="B30">
         <v>2020</v>
       </c>
-      <c r="C27">
+      <c r="C30">
         <v>2027</v>
       </c>
-      <c r="D27">
-        <v>2030</v>
-      </c>
-      <c r="E27">
+      <c r="D30">
+        <v>2031</v>
+      </c>
+      <c r="E30">
         <v>2050</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B28">
-        <f>B24/B25</f>
+      <c r="B31">
+        <f>B27/B24</f>
         <v>0.1000375</v>
       </c>
-      <c r="C28">
-        <f>(B24+'EV charger assumptions'!B9)/Calculations!B25</f>
-        <v>0.41965865943214825</v>
-      </c>
-      <c r="D28">
-        <f>(E28-C28)/(E27-C27)*3+C28</f>
-        <v>0.495355356027955</v>
-      </c>
-      <c r="E28">
+      <c r="C31" cm="1">
+        <f t="array" ref="C31">(TREND(B27:B28,A27:A28,C30)+IIJA!B9)/Calculations!B24</f>
+        <v>0.62964990943214827</v>
+      </c>
+      <c r="D31" cm="1">
+        <f t="array" ref="D31">(TREND(B27:B28,A27:A28,D30)+IIJA!B9+'Inflation Reduction Act'!B23)/Calculations!B24</f>
+        <v>0.86437943919981641</v>
+      </c>
+      <c r="E31">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B29">
+      <c r="B32">
         <f>B19*About!$B$53</f>
         <v>898.05481563188175</v>
       </c>
-      <c r="C29">
-        <f>-667.1*LN(C28)-241.23</f>
-        <v>338.02201174921117</v>
-      </c>
-      <c r="D29">
-        <f>-667.1*LN(D28)-241.23</f>
-        <v>227.39432995486422</v>
-      </c>
-      <c r="E29">
+      <c r="C32">
+        <f>-667.1*LN(C31)-241.23</f>
+        <v>67.364665148257785</v>
+      </c>
+      <c r="D32">
+        <f>MAX(-667.1*LN(D31)-241.23,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
         <v>2020</v>
       </c>
-      <c r="B36">
-        <f>B14*1000+B29</f>
+      <c r="B39">
+        <f>B14*1000+B32</f>
         <v>8780.9012221455905</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row r="40" spans="1:3">
+      <c r="A40">
         <v>2027</v>
       </c>
-      <c r="B37" cm="1">
-        <f t="array" ref="B37">TREND(B14:C14,B7:C7,C27)*1000+C29</f>
-        <v>6349.8416004663277</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2030</v>
-      </c>
-      <c r="B38">
-        <f>C14*1000+D29</f>
-        <v>5437.3452824734923</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="B40" cm="1">
+        <f t="array" ref="B40">TREND(B14:C14,B7:C7,C30)*1000+C32</f>
+        <v>6079.1842538653746</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>2031</v>
+      </c>
+      <c r="B41">
+        <f>C14*1000+D32</f>
+        <v>5209.9509525186277</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
         <v>2050</v>
       </c>
-      <c r="B39">
-        <f>D14*1000+E29</f>
+      <c r="B42">
+        <f>D14*1000+E32</f>
         <v>0</v>
       </c>
     </row>
@@ -2154,29 +2318,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D98A39-3A78-451F-9516-0CF8624C92E2}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -2184,8 +2351,8 @@
         <v>7500000000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="10" t="s">
         <v>63</v>
       </c>
       <c r="B5">
@@ -2193,16 +2360,16 @@
         <v>9375000000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="10" t="s">
         <v>64</v>
       </c>
       <c r="B7">
         <v>24443</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B9" s="3">
@@ -2216,6 +2383,997 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7347CE-ACDC-4498-BA24-2581FCABA72A}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:AL24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="60.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="13" customWidth="1"/>
+    <col min="5" max="6" width="16.140625" style="13" customWidth="1"/>
+    <col min="7" max="11" width="12.5703125" style="13"/>
+    <col min="12" max="12" width="16.42578125" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="12.5703125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:38" ht="14.25" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+    </row>
+    <row r="2" spans="1:38" ht="180">
+      <c r="A2" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:38" ht="14.25" customHeight="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+      <c r="W3" s="17"/>
+      <c r="X3" s="17"/>
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="17"/>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
+      <c r="AC3" s="17"/>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17"/>
+      <c r="AF3" s="17"/>
+      <c r="AG3" s="17"/>
+      <c r="AH3" s="17"/>
+      <c r="AI3" s="17"/>
+      <c r="AJ3" s="17"/>
+      <c r="AK3" s="17"/>
+      <c r="AL3" s="17"/>
+    </row>
+    <row r="4" spans="1:38" ht="14.25" customHeight="1">
+      <c r="A4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+    </row>
+    <row r="5" spans="1:38" ht="14.25" customHeight="1">
+      <c r="A5" s="15"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="17"/>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
+    </row>
+    <row r="6" spans="1:38" ht="14.25" customHeight="1">
+      <c r="A6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="12"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+    </row>
+    <row r="7" spans="1:38" ht="15">
+      <c r="A7" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="17">
+        <v>24443</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+    </row>
+    <row r="8" spans="1:38" ht="15">
+      <c r="A8" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:38" ht="15">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:38" ht="15">
+      <c r="A10" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="19"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
+      <c r="AF10" s="19"/>
+      <c r="AG10" s="19"/>
+      <c r="AH10" s="19"/>
+      <c r="AI10" s="19"/>
+      <c r="AJ10" s="19"/>
+      <c r="AK10" s="19"/>
+      <c r="AL10" s="19"/>
+    </row>
+    <row r="11" spans="1:38" ht="15">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19"/>
+    </row>
+    <row r="12" spans="1:38" ht="30">
+      <c r="A12" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="19"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19"/>
+      <c r="AG12" s="19"/>
+      <c r="AH12" s="19"/>
+      <c r="AI12" s="19"/>
+      <c r="AJ12" s="19"/>
+      <c r="AK12" s="19"/>
+      <c r="AL12" s="19"/>
+    </row>
+    <row r="13" spans="1:38" ht="15">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="19"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19"/>
+      <c r="AG13" s="19"/>
+      <c r="AH13" s="19"/>
+      <c r="AI13" s="19"/>
+      <c r="AJ13" s="19"/>
+      <c r="AK13" s="19"/>
+      <c r="AL13" s="19"/>
+    </row>
+    <row r="14" spans="1:38" ht="15">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
+      <c r="AG14" s="19"/>
+      <c r="AH14" s="19"/>
+      <c r="AI14" s="19"/>
+      <c r="AJ14" s="19"/>
+      <c r="AK14" s="19"/>
+      <c r="AL14" s="19"/>
+    </row>
+    <row r="15" spans="1:38" ht="15">
+      <c r="A15" s="18"/>
+      <c r="B15" s="15">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2023</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2024</v>
+      </c>
+      <c r="E15" s="15">
+        <v>2025</v>
+      </c>
+      <c r="F15" s="15">
+        <v>2026</v>
+      </c>
+      <c r="G15" s="15">
+        <v>2027</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2028</v>
+      </c>
+      <c r="I15" s="15">
+        <v>2029</v>
+      </c>
+      <c r="J15" s="15">
+        <v>2030</v>
+      </c>
+      <c r="K15" s="15">
+        <v>2031</v>
+      </c>
+      <c r="L15" s="15">
+        <v>2032</v>
+      </c>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="19"/>
+      <c r="AL15" s="19"/>
+    </row>
+    <row r="16" spans="1:38" ht="15">
+      <c r="A16" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15">
+        <v>138</v>
+      </c>
+      <c r="D16" s="15">
+        <v>128</v>
+      </c>
+      <c r="E16" s="15">
+        <v>145</v>
+      </c>
+      <c r="F16" s="15">
+        <v>164</v>
+      </c>
+      <c r="G16" s="15">
+        <v>184</v>
+      </c>
+      <c r="H16" s="15">
+        <v>207</v>
+      </c>
+      <c r="I16" s="15">
+        <v>231</v>
+      </c>
+      <c r="J16" s="15">
+        <v>257</v>
+      </c>
+      <c r="K16" s="15">
+        <v>284</v>
+      </c>
+      <c r="L16" s="15"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="19"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="19"/>
+      <c r="AE16" s="19"/>
+      <c r="AF16" s="19"/>
+      <c r="AG16" s="19"/>
+      <c r="AH16" s="19"/>
+      <c r="AI16" s="19"/>
+      <c r="AJ16" s="19"/>
+      <c r="AK16" s="19"/>
+      <c r="AL16" s="19"/>
+    </row>
+    <row r="17" spans="1:38" ht="15">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="19"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="19"/>
+      <c r="AE17" s="19"/>
+      <c r="AF17" s="19"/>
+      <c r="AG17" s="19"/>
+      <c r="AH17" s="19"/>
+      <c r="AI17" s="19"/>
+      <c r="AJ17" s="19"/>
+      <c r="AK17" s="19"/>
+      <c r="AL17" s="19"/>
+    </row>
+    <row r="18" spans="1:38" ht="15">
+      <c r="A18" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="22">
+        <f>C16*0.925</f>
+        <v>127.65</v>
+      </c>
+      <c r="D18" s="22">
+        <f t="shared" ref="D18:L18" si="0">D16*0.925</f>
+        <v>118.4</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" si="0"/>
+        <v>134.125</v>
+      </c>
+      <c r="F18" s="22">
+        <f t="shared" si="0"/>
+        <v>151.70000000000002</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>170.20000000000002</v>
+      </c>
+      <c r="H18" s="22">
+        <f t="shared" si="0"/>
+        <v>191.47500000000002</v>
+      </c>
+      <c r="I18" s="22">
+        <f t="shared" si="0"/>
+        <v>213.67500000000001</v>
+      </c>
+      <c r="J18" s="22">
+        <f t="shared" si="0"/>
+        <v>237.72500000000002</v>
+      </c>
+      <c r="K18" s="22">
+        <f t="shared" si="0"/>
+        <v>262.7</v>
+      </c>
+      <c r="L18" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="19"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="19"/>
+      <c r="AE18" s="19"/>
+      <c r="AF18" s="19"/>
+      <c r="AG18" s="19"/>
+      <c r="AH18" s="19"/>
+      <c r="AI18" s="19"/>
+      <c r="AJ18" s="19"/>
+      <c r="AK18" s="19"/>
+      <c r="AL18" s="19"/>
+    </row>
+    <row r="19" spans="1:38" ht="15">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
+      <c r="AA19" s="19"/>
+      <c r="AB19" s="19"/>
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
+      <c r="AF19" s="19"/>
+      <c r="AG19" s="19"/>
+      <c r="AH19" s="19"/>
+      <c r="AI19" s="19"/>
+      <c r="AJ19" s="19"/>
+      <c r="AK19" s="19"/>
+      <c r="AL19" s="19"/>
+    </row>
+    <row r="20" spans="1:38" ht="15">
+      <c r="B20" s="15">
+        <v>2022</v>
+      </c>
+      <c r="C20" s="15">
+        <v>2023</v>
+      </c>
+      <c r="D20" s="15">
+        <v>2024</v>
+      </c>
+      <c r="E20" s="15">
+        <v>2025</v>
+      </c>
+      <c r="F20" s="15">
+        <v>2026</v>
+      </c>
+      <c r="G20" s="15">
+        <v>2027</v>
+      </c>
+      <c r="H20" s="15">
+        <v>2028</v>
+      </c>
+      <c r="I20" s="15">
+        <v>2029</v>
+      </c>
+      <c r="J20" s="15">
+        <v>2030</v>
+      </c>
+      <c r="K20" s="15">
+        <v>2031</v>
+      </c>
+      <c r="L20" s="15">
+        <v>2032</v>
+      </c>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
+      <c r="AA20" s="19"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
+      <c r="AF20" s="19"/>
+      <c r="AG20" s="19"/>
+      <c r="AH20" s="19"/>
+      <c r="AI20" s="19"/>
+      <c r="AJ20" s="19"/>
+      <c r="AK20" s="19"/>
+      <c r="AL20" s="19"/>
+    </row>
+    <row r="21" spans="1:38" ht="15">
+      <c r="A21" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="15">
+        <v>0</v>
+      </c>
+      <c r="C21" s="22">
+        <f>(C18*10^6)/$B$10/($B$7/$B$8)*$B$12</f>
+        <v>10932.127807552264</v>
+      </c>
+      <c r="D21" s="22">
+        <f t="shared" ref="D21:K21" si="1">(D18*10^6)/$B$10/($B$7/$B$8)*$B$12</f>
+        <v>10139.944633091956</v>
+      </c>
+      <c r="E21" s="22">
+        <f t="shared" si="1"/>
+        <v>11486.656029674483</v>
+      </c>
+      <c r="F21" s="22">
+        <f t="shared" si="1"/>
+        <v>12991.804061149072</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="1"/>
+        <v>14576.17041006969</v>
+      </c>
+      <c r="H21" s="22">
+        <f t="shared" si="1"/>
+        <v>16398.1917113284</v>
+      </c>
+      <c r="I21" s="22">
+        <f t="shared" si="1"/>
+        <v>18299.431330033138</v>
+      </c>
+      <c r="J21" s="22">
+        <f t="shared" si="1"/>
+        <v>20359.107583629942</v>
+      </c>
+      <c r="K21" s="22">
+        <f t="shared" si="1"/>
+        <v>22498.00215467278</v>
+      </c>
+      <c r="L21" s="22">
+        <f>(L18*10^6)/$B$10/$B$7*$B$12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" ht="15">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="19"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19"/>
+      <c r="AG22" s="19"/>
+      <c r="AH22" s="19"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="19"/>
+      <c r="AK22" s="19"/>
+      <c r="AL22" s="19"/>
+    </row>
+    <row r="23" spans="1:38" ht="15">
+      <c r="A23" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="22">
+        <f>SUM(C21:K21)</f>
+        <v>137681.43572120171</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+    </row>
+    <row r="24" spans="1:38" ht="15">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="19"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
+      <c r="AA24" s="19"/>
+      <c r="AB24" s="19"/>
+      <c r="AC24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
+      <c r="AF24" s="19"/>
+      <c r="AG24" s="19"/>
+      <c r="AH24" s="19"/>
+      <c r="AI24" s="19"/>
+      <c r="AJ24" s="19"/>
+      <c r="AK24" s="19"/>
+      <c r="AL24" s="19"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" display="Source: https://www.democrats.senate.gov/imo/media/doc/21-2093.pdf" xr:uid="{30969EEE-E72F-4B62-81B5-E66A5CDAAD8E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -2226,12 +3384,12 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2329,132 +3487,132 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" cm="1">
-        <f t="array" ref="B2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!B1)</f>
-        <v>8780.9012221456505</v>
+        <f t="array" ref="B2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!B1)</f>
+        <v>8780.9012221455341</v>
       </c>
       <c r="C2" s="3" cm="1">
-        <f t="array" ref="C2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!C1)</f>
-        <v>8433.6069904771866</v>
+        <f t="array" ref="C2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!C1)</f>
+        <v>8394.9416552484035</v>
       </c>
       <c r="D2" s="3" cm="1">
-        <f t="array" ref="D2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!D1)</f>
-        <v>8086.3127588086063</v>
+        <f t="array" ref="D2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!D1)</f>
+        <v>8008.982088351273</v>
       </c>
       <c r="E2" s="3" cm="1">
-        <f t="array" ref="E2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!E1)</f>
-        <v>7739.0185271401424</v>
+        <f t="array" ref="E2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!E1)</f>
+        <v>7623.022521454026</v>
       </c>
       <c r="F2" s="3" cm="1">
-        <f t="array" ref="F2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!F1)</f>
-        <v>7391.7242954716785</v>
+        <f t="array" ref="F2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!F1)</f>
+        <v>7237.0629545568954</v>
       </c>
       <c r="G2" s="3" cm="1">
-        <f t="array" ref="G2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!G1)</f>
-        <v>7044.4300638032146</v>
+        <f t="array" ref="G2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!G1)</f>
+        <v>6851.1033876597648</v>
       </c>
       <c r="H2" s="3" cm="1">
-        <f t="array" ref="H2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!H1)</f>
-        <v>6697.1358321347507</v>
+        <f t="array" ref="H2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!H1)</f>
+        <v>6465.1438207625179</v>
       </c>
       <c r="I2" s="3" cm="1">
-        <f t="array" ref="I2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!I1)</f>
-        <v>6349.8416004662868</v>
+        <f t="array" ref="I2">TREND(Calculations!$B$39:$B$40,Calculations!$A$39:$A$40,BRAaCTSC!I1)</f>
+        <v>6079.1842538653873</v>
       </c>
       <c r="J2" s="3" cm="1">
-        <f t="array" ref="J2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!J1)</f>
-        <v>6045.6761611354304</v>
+        <f t="array" ref="J2">TREND(Calculations!$B$40:$B$41,Calculations!$A$40:$A$41,BRAaCTSC!J1)</f>
+        <v>5861.8759285287233</v>
       </c>
       <c r="K2" s="3" cm="1">
-        <f t="array" ref="K2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!K1)</f>
-        <v>5741.5107218045741</v>
+        <f t="array" ref="K2">TREND(Calculations!$B$40:$B$41,Calculations!$A$40:$A$41,BRAaCTSC!K1)</f>
+        <v>5644.5676031920011</v>
       </c>
       <c r="L2" s="3" cm="1">
-        <f t="array" ref="L2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!L1)</f>
-        <v>5437.3452824736014</v>
+        <f t="array" ref="L2">TREND(Calculations!$B$40:$B$41,Calculations!$A$40:$A$41,BRAaCTSC!L1)</f>
+        <v>5427.2592778553371</v>
       </c>
       <c r="M2" s="3" cm="1">
-        <f t="array" ref="M2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!M1)</f>
-        <v>5165.4780183498515</v>
+        <f t="array" ref="M2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!M1)</f>
+        <v>5209.9509525186149</v>
       </c>
       <c r="N2" s="3" cm="1">
-        <f t="array" ref="N2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!N1)</f>
-        <v>4893.610754226218</v>
+        <f t="array" ref="N2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!N1)</f>
+        <v>4935.7430076492019</v>
       </c>
       <c r="O2" s="3" cm="1">
-        <f t="array" ref="O2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!O1)</f>
-        <v>4621.7434901024681</v>
+        <f t="array" ref="O2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!O1)</f>
+        <v>4661.5350627799053</v>
       </c>
       <c r="P2" s="3" cm="1">
-        <f t="array" ref="P2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!P1)</f>
-        <v>4349.8762259788346</v>
+        <f t="array" ref="P2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!P1)</f>
+        <v>4387.3271179104922</v>
       </c>
       <c r="Q2" s="3" cm="1">
-        <f t="array" ref="Q2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Q1)</f>
-        <v>4078.0089618552011</v>
+        <f t="array" ref="Q2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!Q1)</f>
+        <v>4113.1191730410792</v>
       </c>
       <c r="R2" s="3" cm="1">
-        <f t="array" ref="R2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!R1)</f>
-        <v>3806.1416977314511</v>
+        <f t="array" ref="R2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!R1)</f>
+        <v>3838.9112281716662</v>
       </c>
       <c r="S2" s="3" cm="1">
-        <f t="array" ref="S2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!S1)</f>
-        <v>3534.2744336078176</v>
+        <f t="array" ref="S2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!S1)</f>
+        <v>3564.7032833022531</v>
       </c>
       <c r="T2" s="3" cm="1">
-        <f t="array" ref="T2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!T1)</f>
-        <v>3262.4071694841841</v>
+        <f t="array" ref="T2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!T1)</f>
+        <v>3290.4953384328401</v>
       </c>
       <c r="U2" s="3" cm="1">
-        <f t="array" ref="U2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!U1)</f>
-        <v>2990.5399053604342</v>
+        <f t="array" ref="U2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!U1)</f>
+        <v>3016.287393563427</v>
       </c>
       <c r="V2" s="3" cm="1">
-        <f t="array" ref="V2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!V1)</f>
-        <v>2718.6726412368007</v>
+        <f t="array" ref="V2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!V1)</f>
+        <v>2742.079448694014</v>
       </c>
       <c r="W2" s="3" cm="1">
-        <f t="array" ref="W2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!W1)</f>
-        <v>2446.8053771130508</v>
+        <f t="array" ref="W2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!W1)</f>
+        <v>2467.8715038246009</v>
       </c>
       <c r="X2" s="3" cm="1">
-        <f t="array" ref="X2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!X1)</f>
-        <v>2174.9381129894173</v>
+        <f t="array" ref="X2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!X1)</f>
+        <v>2193.6635589551879</v>
       </c>
       <c r="Y2" s="3" cm="1">
-        <f t="array" ref="Y2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Y1)</f>
-        <v>1903.0708488657838</v>
+        <f t="array" ref="Y2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!Y1)</f>
+        <v>1919.4556140858913</v>
       </c>
       <c r="Z2" s="3" cm="1">
-        <f t="array" ref="Z2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Z1)</f>
-        <v>1631.2035847420339</v>
+        <f t="array" ref="Z2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!Z1)</f>
+        <v>1645.2476692164782</v>
       </c>
       <c r="AA2" s="3" cm="1">
-        <f t="array" ref="AA2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AA1)</f>
-        <v>1359.3363206184004</v>
+        <f t="array" ref="AA2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AA1)</f>
+        <v>1371.0397243470652</v>
       </c>
       <c r="AB2" s="3" cm="1">
-        <f t="array" ref="AB2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AB1)</f>
-        <v>1087.4690564947668</v>
+        <f t="array" ref="AB2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AB1)</f>
+        <v>1096.8317794776522</v>
       </c>
       <c r="AC2" s="3" cm="1">
-        <f t="array" ref="AC2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AC1)</f>
-        <v>815.60179237101693</v>
+        <f t="array" ref="AC2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AC1)</f>
+        <v>822.62383460823912</v>
       </c>
       <c r="AD2" s="3" cm="1">
-        <f t="array" ref="AD2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AD1)</f>
-        <v>543.73452824738342</v>
+        <f t="array" ref="AD2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AD1)</f>
+        <v>548.41588973882608</v>
       </c>
       <c r="AE2" s="3" cm="1">
-        <f t="array" ref="AE2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AE1)</f>
-        <v>271.86726412374992</v>
+        <f t="array" ref="AE2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AE1)</f>
+        <v>274.20794486941304</v>
       </c>
       <c r="AF2" s="3" cm="1">
-        <f t="array" ref="AF2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AF1)</f>
+        <f t="array" ref="AF2">TREND(Calculations!$B$41:$B$42,Calculations!$A$41:$A$42,BRAaCTSC!AF1)</f>
         <v>0</v>
       </c>
       <c r="AG2" s="3"/>

</xml_diff>